<commit_message>
Grosse mise à jour (intérieur du code)
</commit_message>
<xml_diff>
--- a/Répartition.xlsx
+++ b/Répartition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\itsia\Documents\IUT\Semestre 2\Projet tut\Tâches\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Travail\1er année DUT\Projets\Projet tutoré S2\projetTutS2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{439D83A6-F9D7-4B18-826D-2F1814347F49}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7B9ED19-80C8-45D7-8204-B640EE95AA2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16995" yWindow="6555" windowWidth="28800" windowHeight="11385" xr2:uid="{036A9EC5-0052-46C3-A001-39F17668F270}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{036A9EC5-0052-46C3-A001-39F17668F270}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="73">
   <si>
     <t>nom</t>
   </si>
@@ -241,13 +243,22 @@
   </si>
   <si>
     <t>Ecrire ActiviesWindow::ActivitiesWindow</t>
+  </si>
+  <si>
+    <t>Etat</t>
+  </si>
+  <si>
+    <t>✓</t>
+  </si>
+  <si>
+    <t>∼</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -268,8 +279,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="20"/>
+      <color theme="9" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="7" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="19">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -378,6 +403,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -443,7 +480,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -503,21 +540,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -537,6 +559,33 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -865,10 +914,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFC8A138-2D9A-4417-92BC-D27501CE0120}">
-  <dimension ref="A1:M56"/>
+  <dimension ref="A1:Q56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43:F55"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -883,16 +932,16 @@
     <col min="13" max="13" width="40" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:17" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="J1">
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="K1">
         <v>43</v>
       </c>
       <c r="L1" s="16"/>
@@ -900,7 +949,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -919,17 +968,20 @@
       <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="36" t="s">
+      <c r="G2" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="8"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="L2" s="34"/>
       <c r="M2" s="19" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -945,19 +997,21 @@
       <c r="E3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="25">
+      <c r="F3" s="37">
         <f>SUM(B3:B13)</f>
         <v>40</v>
       </c>
-      <c r="G3" s="29"/>
+      <c r="G3" s="24"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
-      <c r="J3" s="21"/>
+      <c r="J3" s="35" t="s">
+        <v>71</v>
+      </c>
       <c r="M3" s="18" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
@@ -973,16 +1027,18 @@
       <c r="E4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="26"/>
-      <c r="G4" s="30"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="25"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
-      <c r="J4" s="21"/>
-      <c r="M4" s="32" t="s">
+      <c r="J4" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="M4" s="27" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
@@ -998,16 +1054,21 @@
       <c r="E5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="26"/>
-      <c r="G5" s="31"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="26"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
-      <c r="J5" s="21"/>
+      <c r="J5" s="36" t="s">
+        <v>72</v>
+      </c>
       <c r="M5" s="20" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q5" s="36" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
@@ -1023,16 +1084,21 @@
       <c r="E6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="26"/>
-      <c r="G6" s="28"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="23"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
-      <c r="J6" s="21"/>
-      <c r="M6" s="35" t="s">
+      <c r="J6" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="M6" s="30" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q6" s="35" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
@@ -1048,16 +1114,18 @@
       <c r="E7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="26"/>
-      <c r="G7" s="33"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="28"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
-      <c r="J7" s="21"/>
+      <c r="J7" s="35" t="s">
+        <v>71</v>
+      </c>
       <c r="M7" s="17" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -1073,13 +1141,15 @@
       <c r="E8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="26"/>
-      <c r="G8" s="34"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="29"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
-      <c r="J8" s="21"/>
-    </row>
-    <row r="9" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J8" s="35" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -1095,13 +1165,15 @@
       <c r="E9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="26"/>
-      <c r="G9" s="31"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="26"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
-      <c r="J9" s="21"/>
-    </row>
-    <row r="10" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J9" s="35" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -1117,13 +1189,15 @@
       <c r="E10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="26"/>
-      <c r="G10" s="29"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="24"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
-      <c r="J10" s="21"/>
-    </row>
-    <row r="11" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J10" s="35" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>13</v>
       </c>
@@ -1139,13 +1213,15 @@
       <c r="E11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="26"/>
-      <c r="G11" s="30"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="25"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
-      <c r="J11" s="21"/>
-    </row>
-    <row r="12" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J11" s="35" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
@@ -1161,13 +1237,13 @@
       <c r="E12" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="26"/>
-      <c r="G12" s="34"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="29"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
-      <c r="J12" s="21"/>
-    </row>
-    <row r="13" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" spans="1:17" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>14</v>
       </c>
@@ -1183,21 +1259,23 @@
       <c r="E13" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="27"/>
-      <c r="G13" s="33"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="28"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
-      <c r="J13" s="21"/>
-    </row>
-    <row r="16" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="23" t="s">
+      <c r="J13" s="35" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="23"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
+      <c r="B16" s="40"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
       <c r="M16" s="22" t="s">
         <v>68</v>
       </c>
@@ -1221,12 +1299,14 @@
       <c r="F17" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G17" s="36" t="s">
+      <c r="G17" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="H17" s="36"/>
-      <c r="I17" s="36"/>
-      <c r="J17" s="8"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="31" t="s">
+        <v>70</v>
+      </c>
       <c r="M17" s="19" t="s">
         <v>61</v>
       </c>
@@ -1247,14 +1327,16 @@
       <c r="E18" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F18" s="24">
+      <c r="F18" s="41">
         <f>SUM(B18:B26)</f>
         <v>24</v>
       </c>
-      <c r="G18" s="30"/>
-      <c r="H18" s="34"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="29"/>
       <c r="I18" s="3"/>
-      <c r="J18" s="21"/>
+      <c r="J18" s="35" t="s">
+        <v>71</v>
+      </c>
       <c r="M18" s="18" t="s">
         <v>62</v>
       </c>
@@ -1275,12 +1357,14 @@
       <c r="E19" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F19" s="24"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="31"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="26"/>
       <c r="I19" s="3"/>
-      <c r="J19" s="21"/>
-      <c r="M19" s="32" t="s">
+      <c r="J19" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="M19" s="27" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1300,11 +1384,13 @@
       <c r="E20" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="F20" s="24"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="31"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="26"/>
       <c r="I20" s="3"/>
-      <c r="J20" s="21"/>
+      <c r="J20" s="35" t="s">
+        <v>71</v>
+      </c>
       <c r="M20" s="20" t="s">
         <v>64</v>
       </c>
@@ -1325,12 +1411,14 @@
       <c r="E21" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="F21" s="24"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="31"/>
+      <c r="F21" s="41"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="26"/>
       <c r="I21" s="3"/>
-      <c r="J21" s="21"/>
-      <c r="M21" s="35" t="s">
+      <c r="J21" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="M21" s="30" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1350,11 +1438,13 @@
       <c r="E22" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="F22" s="24"/>
-      <c r="G22" s="29"/>
-      <c r="H22" s="28"/>
+      <c r="F22" s="41"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="23"/>
       <c r="I22" s="3"/>
-      <c r="J22" s="21"/>
+      <c r="J22" s="35" t="s">
+        <v>71</v>
+      </c>
       <c r="M22" s="17" t="s">
         <v>66</v>
       </c>
@@ -1375,11 +1465,13 @@
       <c r="E23" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="F23" s="24"/>
-      <c r="G23" s="30"/>
-      <c r="H23" s="38"/>
+      <c r="F23" s="41"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="33"/>
       <c r="I23" s="3"/>
-      <c r="J23" s="21"/>
+      <c r="J23" s="35" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="24" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
@@ -1397,11 +1489,13 @@
       <c r="E24" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="F24" s="24"/>
-      <c r="G24" s="29"/>
-      <c r="H24" s="28"/>
+      <c r="F24" s="41"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="23"/>
       <c r="I24" s="3"/>
-      <c r="J24" s="21"/>
+      <c r="J24" s="35" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="25" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
@@ -1419,11 +1513,11 @@
       <c r="E25" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F25" s="24"/>
-      <c r="G25" s="29"/>
-      <c r="H25" s="28"/>
+      <c r="F25" s="41"/>
+      <c r="G25" s="24"/>
+      <c r="H25" s="23"/>
       <c r="I25" s="3"/>
-      <c r="J25" s="21"/>
+      <c r="J25" s="3"/>
     </row>
     <row r="26" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
@@ -1441,11 +1535,13 @@
       <c r="E26" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F26" s="24"/>
-      <c r="G26" s="30"/>
-      <c r="H26" s="34"/>
+      <c r="F26" s="41"/>
+      <c r="G26" s="25"/>
+      <c r="H26" s="29"/>
       <c r="I26" s="3"/>
-      <c r="J26" s="21"/>
+      <c r="J26" s="35" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="27" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
@@ -1454,10 +1550,10 @@
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
       <c r="F27" s="9"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="32"/>
+      <c r="I27" s="32"/>
+      <c r="J27" s="32"/>
     </row>
     <row r="28" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
@@ -1466,20 +1562,20 @@
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
       <c r="F28" s="9"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
     </row>
     <row r="29" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="23" t="s">
+      <c r="A29" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="B29" s="23"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
       <c r="M29" s="22" t="s">
         <v>68</v>
       </c>
@@ -1503,12 +1599,14 @@
       <c r="F30" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G30" s="36" t="s">
+      <c r="G30" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="H30" s="36"/>
-      <c r="I30" s="36"/>
-      <c r="J30" s="8"/>
+      <c r="H30" s="42"/>
+      <c r="I30" s="42"/>
+      <c r="J30" s="31" t="s">
+        <v>70</v>
+      </c>
       <c r="M30" s="19" t="s">
         <v>61</v>
       </c>
@@ -1529,14 +1627,16 @@
       <c r="E31" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F31" s="24">
+      <c r="F31" s="41">
         <f>SUM(B31:B38)</f>
         <v>37</v>
       </c>
-      <c r="G31" s="30"/>
-      <c r="H31" s="34"/>
-      <c r="I31" s="33"/>
-      <c r="J31" s="21"/>
+      <c r="G31" s="25"/>
+      <c r="H31" s="29"/>
+      <c r="I31" s="28"/>
+      <c r="J31" s="35" t="s">
+        <v>71</v>
+      </c>
       <c r="M31" s="18" t="s">
         <v>62</v>
       </c>
@@ -1557,12 +1657,14 @@
       <c r="E32" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="F32" s="24"/>
-      <c r="G32" s="30"/>
-      <c r="H32" s="34"/>
-      <c r="I32" s="33"/>
-      <c r="J32" s="21"/>
-      <c r="M32" s="32" t="s">
+      <c r="F32" s="41"/>
+      <c r="G32" s="25"/>
+      <c r="H32" s="29"/>
+      <c r="I32" s="28"/>
+      <c r="J32" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="M32" s="27" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1582,11 +1684,13 @@
       <c r="E33" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="F33" s="24"/>
-      <c r="G33" s="30"/>
-      <c r="H33" s="34"/>
-      <c r="I33" s="33"/>
-      <c r="J33" s="21"/>
+      <c r="F33" s="41"/>
+      <c r="G33" s="25"/>
+      <c r="H33" s="29"/>
+      <c r="I33" s="28"/>
+      <c r="J33" s="35" t="s">
+        <v>71</v>
+      </c>
       <c r="M33" s="20" t="s">
         <v>64</v>
       </c>
@@ -1607,12 +1711,12 @@
       <c r="E34" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="F34" s="24"/>
-      <c r="G34" s="29"/>
-      <c r="H34" s="28"/>
-      <c r="I34" s="31"/>
-      <c r="J34" s="21"/>
-      <c r="M34" s="35" t="s">
+      <c r="F34" s="41"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="23"/>
+      <c r="I34" s="26"/>
+      <c r="J34" s="3"/>
+      <c r="M34" s="30" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1632,11 +1736,11 @@
       <c r="E35" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F35" s="24"/>
-      <c r="G35" s="29"/>
-      <c r="H35" s="28"/>
-      <c r="I35" s="31"/>
-      <c r="J35" s="21"/>
+      <c r="F35" s="41"/>
+      <c r="G35" s="24"/>
+      <c r="H35" s="23"/>
+      <c r="I35" s="26"/>
+      <c r="J35" s="3"/>
       <c r="M35" s="17" t="s">
         <v>66</v>
       </c>
@@ -1657,11 +1761,11 @@
       <c r="E36" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F36" s="24"/>
-      <c r="G36" s="30"/>
-      <c r="H36" s="34"/>
-      <c r="I36" s="33"/>
-      <c r="J36" s="21"/>
+      <c r="F36" s="41"/>
+      <c r="G36" s="25"/>
+      <c r="H36" s="29"/>
+      <c r="I36" s="28"/>
+      <c r="J36" s="3"/>
     </row>
     <row r="37" spans="1:13" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
@@ -1679,11 +1783,11 @@
       <c r="E37" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F37" s="24"/>
-      <c r="G37" s="29"/>
-      <c r="H37" s="28"/>
-      <c r="I37" s="31"/>
-      <c r="J37" s="21"/>
+      <c r="F37" s="41"/>
+      <c r="G37" s="24"/>
+      <c r="H37" s="23"/>
+      <c r="I37" s="26"/>
+      <c r="J37" s="3"/>
     </row>
     <row r="38" spans="1:13" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
@@ -1701,11 +1805,11 @@
       <c r="E38" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="F38" s="24"/>
-      <c r="G38" s="29"/>
-      <c r="H38" s="28"/>
-      <c r="I38" s="31"/>
-      <c r="J38" s="21"/>
+      <c r="F38" s="41"/>
+      <c r="G38" s="24"/>
+      <c r="H38" s="23"/>
+      <c r="I38" s="26"/>
+      <c r="J38" s="3"/>
     </row>
     <row r="39" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="8"/>
@@ -1714,30 +1818,30 @@
       <c r="D39" s="8"/>
       <c r="E39" s="8"/>
       <c r="F39" s="9"/>
-      <c r="G39" s="37"/>
+      <c r="G39" s="32"/>
       <c r="H39" s="21"/>
       <c r="I39" s="21"/>
       <c r="J39" s="21"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="G40" s="37"/>
-      <c r="H40" s="37"/>
-      <c r="I40" s="37"/>
-      <c r="J40" s="37"/>
+      <c r="G40" s="32"/>
+      <c r="H40" s="32"/>
+      <c r="I40" s="32"/>
+      <c r="J40" s="32"/>
     </row>
     <row r="41" spans="1:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="23" t="s">
+      <c r="A41" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="B41" s="23"/>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23"/>
-      <c r="E41" s="23"/>
-      <c r="F41" s="23"/>
-      <c r="G41" s="37"/>
-      <c r="H41" s="37"/>
-      <c r="I41" s="37"/>
-      <c r="J41" s="37"/>
+      <c r="B41" s="40"/>
+      <c r="C41" s="40"/>
+      <c r="D41" s="40"/>
+      <c r="E41" s="40"/>
+      <c r="F41" s="40"/>
+      <c r="G41" s="32"/>
+      <c r="H41" s="32"/>
+      <c r="I41" s="32"/>
+      <c r="J41" s="32"/>
       <c r="M41" s="22" t="s">
         <v>68</v>
       </c>
@@ -1761,12 +1865,14 @@
       <c r="F42" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G42" s="36" t="s">
+      <c r="G42" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="H42" s="36"/>
-      <c r="I42" s="36"/>
-      <c r="J42" s="8"/>
+      <c r="H42" s="42"/>
+      <c r="I42" s="42"/>
+      <c r="J42" s="31" t="s">
+        <v>70</v>
+      </c>
       <c r="M42" s="19" t="s">
         <v>61</v>
       </c>
@@ -1787,14 +1893,14 @@
       <c r="E43" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="F43" s="25">
+      <c r="F43" s="37">
         <f>SUM(B43:B55)</f>
         <v>56</v>
       </c>
-      <c r="G43" s="30"/>
-      <c r="H43" s="34"/>
-      <c r="I43" s="31"/>
-      <c r="J43" s="37"/>
+      <c r="G43" s="25"/>
+      <c r="H43" s="29"/>
+      <c r="I43" s="26"/>
+      <c r="J43" s="3"/>
       <c r="M43" s="18" t="s">
         <v>62</v>
       </c>
@@ -1815,12 +1921,12 @@
       <c r="E44" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="F44" s="26"/>
-      <c r="G44" s="29"/>
-      <c r="H44" s="28"/>
-      <c r="I44" s="33"/>
-      <c r="J44" s="21"/>
-      <c r="M44" s="32" t="s">
+      <c r="F44" s="38"/>
+      <c r="G44" s="24"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="28"/>
+      <c r="J44" s="3"/>
+      <c r="M44" s="27" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1840,11 +1946,11 @@
       <c r="E45" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="F45" s="26"/>
-      <c r="G45" s="29"/>
-      <c r="H45" s="28"/>
-      <c r="I45" s="33"/>
-      <c r="J45" s="21"/>
+      <c r="F45" s="38"/>
+      <c r="G45" s="24"/>
+      <c r="H45" s="23"/>
+      <c r="I45" s="28"/>
+      <c r="J45" s="3"/>
       <c r="M45" s="20" t="s">
         <v>64</v>
       </c>
@@ -1865,12 +1971,12 @@
       <c r="E46" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="F46" s="26"/>
-      <c r="G46" s="29"/>
-      <c r="H46" s="28"/>
-      <c r="I46" s="33"/>
-      <c r="J46" s="21"/>
-      <c r="M46" s="35" t="s">
+      <c r="F46" s="38"/>
+      <c r="G46" s="24"/>
+      <c r="H46" s="23"/>
+      <c r="I46" s="28"/>
+      <c r="J46" s="3"/>
+      <c r="M46" s="30" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1890,11 +1996,11 @@
       <c r="E47" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="F47" s="26"/>
-      <c r="G47" s="30"/>
-      <c r="H47" s="34"/>
-      <c r="I47" s="31"/>
-      <c r="J47" s="21"/>
+      <c r="F47" s="38"/>
+      <c r="G47" s="25"/>
+      <c r="H47" s="29"/>
+      <c r="I47" s="26"/>
+      <c r="J47" s="3"/>
       <c r="M47" s="17" t="s">
         <v>66</v>
       </c>
@@ -1915,11 +2021,11 @@
       <c r="E48" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="F48" s="26"/>
-      <c r="G48" s="29"/>
-      <c r="H48" s="28"/>
-      <c r="I48" s="33"/>
-      <c r="J48" s="21"/>
+      <c r="F48" s="38"/>
+      <c r="G48" s="24"/>
+      <c r="H48" s="23"/>
+      <c r="I48" s="28"/>
+      <c r="J48" s="3"/>
     </row>
     <row r="49" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
@@ -1937,11 +2043,11 @@
       <c r="E49" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="F49" s="26"/>
-      <c r="G49" s="30"/>
-      <c r="H49" s="34"/>
-      <c r="I49" s="31"/>
-      <c r="J49" s="21"/>
+      <c r="F49" s="38"/>
+      <c r="G49" s="25"/>
+      <c r="H49" s="29"/>
+      <c r="I49" s="26"/>
+      <c r="J49" s="3"/>
     </row>
     <row r="50" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
@@ -1959,11 +2065,11 @@
       <c r="E50" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="F50" s="26"/>
-      <c r="G50" s="29"/>
-      <c r="H50" s="28"/>
-      <c r="I50" s="33"/>
-      <c r="J50" s="21"/>
+      <c r="F50" s="38"/>
+      <c r="G50" s="24"/>
+      <c r="H50" s="23"/>
+      <c r="I50" s="28"/>
+      <c r="J50" s="3"/>
     </row>
     <row r="51" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
@@ -1981,11 +2087,11 @@
       <c r="E51" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="F51" s="26"/>
-      <c r="G51" s="30"/>
-      <c r="H51" s="34"/>
-      <c r="I51" s="31"/>
-      <c r="J51" s="21"/>
+      <c r="F51" s="38"/>
+      <c r="G51" s="25"/>
+      <c r="H51" s="29"/>
+      <c r="I51" s="26"/>
+      <c r="J51" s="3"/>
     </row>
     <row r="52" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="14" t="s">
@@ -2003,11 +2109,11 @@
       <c r="E52" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="F52" s="26"/>
-      <c r="G52" s="29"/>
-      <c r="H52" s="28"/>
-      <c r="I52" s="33"/>
-      <c r="J52" s="21"/>
+      <c r="F52" s="38"/>
+      <c r="G52" s="24"/>
+      <c r="H52" s="23"/>
+      <c r="I52" s="28"/>
+      <c r="J52" s="3"/>
     </row>
     <row r="53" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
@@ -2025,11 +2131,11 @@
       <c r="E53" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="F53" s="26"/>
-      <c r="G53" s="30"/>
-      <c r="H53" s="34"/>
-      <c r="I53" s="31"/>
-      <c r="J53" s="21"/>
+      <c r="F53" s="38"/>
+      <c r="G53" s="25"/>
+      <c r="H53" s="29"/>
+      <c r="I53" s="26"/>
+      <c r="J53" s="3"/>
     </row>
     <row r="54" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="14" t="s">
@@ -2047,11 +2153,11 @@
       <c r="E54" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="F54" s="26"/>
-      <c r="G54" s="30"/>
-      <c r="H54" s="34"/>
-      <c r="I54" s="31"/>
-      <c r="J54" s="21"/>
+      <c r="F54" s="38"/>
+      <c r="G54" s="25"/>
+      <c r="H54" s="29"/>
+      <c r="I54" s="26"/>
+      <c r="J54" s="3"/>
     </row>
     <row r="55" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="14" t="s">
@@ -2069,11 +2175,11 @@
       <c r="E55" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="F55" s="27"/>
-      <c r="G55" s="29"/>
-      <c r="H55" s="28"/>
-      <c r="I55" s="33"/>
-      <c r="J55" s="21"/>
+      <c r="F55" s="39"/>
+      <c r="G55" s="24"/>
+      <c r="H55" s="23"/>
+      <c r="I55" s="28"/>
+      <c r="J55" s="3"/>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>

</xml_diff>

<commit_message>
Mise en place liste des projets
</commit_message>
<xml_diff>
--- a/Répartition.xlsx
+++ b/Répartition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Travail\1er année DUT\Projets\Projet tutoré S2\projetTutS2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F6115EF-0878-4BCA-9287-8AF75F123235}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A99E4171-8C56-4C99-85B6-125B19ED4C30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{036A9EC5-0052-46C3-A001-39F17668F270}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{036A9EC5-0052-46C3-A001-39F17668F270}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -568,22 +568,22 @@
     <xf numFmtId="0" fontId="4" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -933,14 +933,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
       <c r="K1">
         <v>43</v>
       </c>
@@ -968,11 +968,11 @@
       <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="37" t="s">
+      <c r="G2" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
       <c r="J2" s="31" t="s">
         <v>70</v>
       </c>
@@ -997,7 +997,7 @@
       <c r="E3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="40">
+      <c r="F3" s="37">
         <f>SUM(B3:B13)</f>
         <v>40</v>
       </c>
@@ -1027,7 +1027,7 @@
       <c r="E4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="41"/>
+      <c r="F4" s="38"/>
       <c r="G4" s="25"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
@@ -1054,7 +1054,7 @@
       <c r="E5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="41"/>
+      <c r="F5" s="38"/>
       <c r="G5" s="26"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -1084,7 +1084,7 @@
       <c r="E6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="41"/>
+      <c r="F6" s="38"/>
       <c r="G6" s="23"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
@@ -1114,7 +1114,7 @@
       <c r="E7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="41"/>
+      <c r="F7" s="38"/>
       <c r="G7" s="28"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
@@ -1141,7 +1141,7 @@
       <c r="E8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="41"/>
+      <c r="F8" s="38"/>
       <c r="G8" s="29"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
@@ -1165,7 +1165,7 @@
       <c r="E9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="41"/>
+      <c r="F9" s="38"/>
       <c r="G9" s="26"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
@@ -1189,7 +1189,7 @@
       <c r="E10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="41"/>
+      <c r="F10" s="38"/>
       <c r="G10" s="24"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
@@ -1213,7 +1213,7 @@
       <c r="E11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="41"/>
+      <c r="F11" s="38"/>
       <c r="G11" s="25"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
@@ -1237,7 +1237,7 @@
       <c r="E12" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="41"/>
+      <c r="F12" s="38"/>
       <c r="G12" s="29"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
@@ -1259,7 +1259,7 @@
       <c r="E13" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="42"/>
+      <c r="F13" s="39"/>
       <c r="G13" s="28"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
@@ -1268,14 +1268,14 @@
       </c>
     </row>
     <row r="16" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="38" t="s">
+      <c r="A16" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="38"/>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
+      <c r="B16" s="40"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
       <c r="M16" s="22" t="s">
         <v>68</v>
       </c>
@@ -1299,11 +1299,11 @@
       <c r="F17" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G17" s="37" t="s">
+      <c r="G17" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="H17" s="37"/>
-      <c r="I17" s="37"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
       <c r="J17" s="31" t="s">
         <v>70</v>
       </c>
@@ -1327,7 +1327,7 @@
       <c r="E18" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F18" s="39">
+      <c r="F18" s="41">
         <f>SUM(B18:B26)</f>
         <v>24</v>
       </c>
@@ -1357,7 +1357,7 @@
       <c r="E19" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F19" s="39"/>
+      <c r="F19" s="41"/>
       <c r="G19" s="28"/>
       <c r="H19" s="26"/>
       <c r="I19" s="3"/>
@@ -1384,7 +1384,7 @@
       <c r="E20" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="F20" s="39"/>
+      <c r="F20" s="41"/>
       <c r="G20" s="28"/>
       <c r="H20" s="26"/>
       <c r="I20" s="3"/>
@@ -1411,7 +1411,7 @@
       <c r="E21" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="F21" s="39"/>
+      <c r="F21" s="41"/>
       <c r="G21" s="28"/>
       <c r="H21" s="26"/>
       <c r="I21" s="3"/>
@@ -1438,7 +1438,7 @@
       <c r="E22" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="F22" s="39"/>
+      <c r="F22" s="41"/>
       <c r="G22" s="24"/>
       <c r="H22" s="23"/>
       <c r="I22" s="3"/>
@@ -1465,7 +1465,7 @@
       <c r="E23" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="F23" s="39"/>
+      <c r="F23" s="41"/>
       <c r="G23" s="25"/>
       <c r="H23" s="33"/>
       <c r="I23" s="3"/>
@@ -1489,7 +1489,7 @@
       <c r="E24" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="F24" s="39"/>
+      <c r="F24" s="41"/>
       <c r="G24" s="24"/>
       <c r="H24" s="23"/>
       <c r="I24" s="3"/>
@@ -1513,7 +1513,7 @@
       <c r="E25" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F25" s="39"/>
+      <c r="F25" s="41"/>
       <c r="G25" s="24"/>
       <c r="H25" s="23"/>
       <c r="I25" s="3"/>
@@ -1535,7 +1535,7 @@
       <c r="E26" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F26" s="39"/>
+      <c r="F26" s="41"/>
       <c r="G26" s="25"/>
       <c r="H26" s="29"/>
       <c r="I26" s="3"/>
@@ -1568,14 +1568,14 @@
       <c r="J28" s="32"/>
     </row>
     <row r="29" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="38" t="s">
+      <c r="A29" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="B29" s="38"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
       <c r="M29" s="22" t="s">
         <v>68</v>
       </c>
@@ -1599,11 +1599,11 @@
       <c r="F30" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G30" s="37" t="s">
+      <c r="G30" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="H30" s="37"/>
-      <c r="I30" s="37"/>
+      <c r="H30" s="42"/>
+      <c r="I30" s="42"/>
       <c r="J30" s="31" t="s">
         <v>70</v>
       </c>
@@ -1627,7 +1627,7 @@
       <c r="E31" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F31" s="39">
+      <c r="F31" s="41">
         <f>SUM(B31:B38)</f>
         <v>37</v>
       </c>
@@ -1657,7 +1657,7 @@
       <c r="E32" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="F32" s="39"/>
+      <c r="F32" s="41"/>
       <c r="G32" s="25"/>
       <c r="H32" s="29"/>
       <c r="I32" s="28"/>
@@ -1684,7 +1684,7 @@
       <c r="E33" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="F33" s="39"/>
+      <c r="F33" s="41"/>
       <c r="G33" s="25"/>
       <c r="H33" s="29"/>
       <c r="I33" s="28"/>
@@ -1711,12 +1711,12 @@
       <c r="E34" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="F34" s="39"/>
+      <c r="F34" s="41"/>
       <c r="G34" s="24"/>
       <c r="H34" s="23"/>
       <c r="I34" s="26"/>
-      <c r="J34" s="36" t="s">
-        <v>72</v>
+      <c r="J34" s="35" t="s">
+        <v>71</v>
       </c>
       <c r="M34" s="30" t="s">
         <v>65</v>
@@ -1738,7 +1738,7 @@
       <c r="E35" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F35" s="39"/>
+      <c r="F35" s="41"/>
       <c r="G35" s="24"/>
       <c r="H35" s="23"/>
       <c r="I35" s="26"/>
@@ -1763,7 +1763,7 @@
       <c r="E36" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F36" s="39"/>
+      <c r="F36" s="41"/>
       <c r="G36" s="25"/>
       <c r="H36" s="29"/>
       <c r="I36" s="28"/>
@@ -1785,7 +1785,7 @@
       <c r="E37" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F37" s="39"/>
+      <c r="F37" s="41"/>
       <c r="G37" s="24"/>
       <c r="H37" s="23"/>
       <c r="I37" s="26"/>
@@ -1807,7 +1807,7 @@
       <c r="E38" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="F38" s="39"/>
+      <c r="F38" s="41"/>
       <c r="G38" s="24"/>
       <c r="H38" s="23"/>
       <c r="I38" s="26"/>
@@ -1832,14 +1832,14 @@
       <c r="J40" s="32"/>
     </row>
     <row r="41" spans="1:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="38" t="s">
+      <c r="A41" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="B41" s="38"/>
-      <c r="C41" s="38"/>
-      <c r="D41" s="38"/>
-      <c r="E41" s="38"/>
-      <c r="F41" s="38"/>
+      <c r="B41" s="40"/>
+      <c r="C41" s="40"/>
+      <c r="D41" s="40"/>
+      <c r="E41" s="40"/>
+      <c r="F41" s="40"/>
       <c r="G41" s="32"/>
       <c r="H41" s="32"/>
       <c r="I41" s="32"/>
@@ -1867,11 +1867,11 @@
       <c r="F42" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G42" s="37" t="s">
+      <c r="G42" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="H42" s="37"/>
-      <c r="I42" s="37"/>
+      <c r="H42" s="42"/>
+      <c r="I42" s="42"/>
       <c r="J42" s="31" t="s">
         <v>70</v>
       </c>
@@ -1895,7 +1895,7 @@
       <c r="E43" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="F43" s="40">
+      <c r="F43" s="37">
         <f>SUM(B43:B55)</f>
         <v>56</v>
       </c>
@@ -1923,7 +1923,7 @@
       <c r="E44" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="F44" s="41"/>
+      <c r="F44" s="38"/>
       <c r="G44" s="24"/>
       <c r="H44" s="23"/>
       <c r="I44" s="28"/>
@@ -1948,7 +1948,7 @@
       <c r="E45" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="F45" s="41"/>
+      <c r="F45" s="38"/>
       <c r="G45" s="24"/>
       <c r="H45" s="23"/>
       <c r="I45" s="28"/>
@@ -1973,7 +1973,7 @@
       <c r="E46" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="F46" s="41"/>
+      <c r="F46" s="38"/>
       <c r="G46" s="24"/>
       <c r="H46" s="23"/>
       <c r="I46" s="28"/>
@@ -1998,7 +1998,7 @@
       <c r="E47" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="F47" s="41"/>
+      <c r="F47" s="38"/>
       <c r="G47" s="25"/>
       <c r="H47" s="29"/>
       <c r="I47" s="26"/>
@@ -2023,7 +2023,7 @@
       <c r="E48" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="F48" s="41"/>
+      <c r="F48" s="38"/>
       <c r="G48" s="24"/>
       <c r="H48" s="23"/>
       <c r="I48" s="28"/>
@@ -2045,7 +2045,7 @@
       <c r="E49" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="F49" s="41"/>
+      <c r="F49" s="38"/>
       <c r="G49" s="25"/>
       <c r="H49" s="29"/>
       <c r="I49" s="26"/>
@@ -2067,7 +2067,7 @@
       <c r="E50" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="F50" s="41"/>
+      <c r="F50" s="38"/>
       <c r="G50" s="24"/>
       <c r="H50" s="23"/>
       <c r="I50" s="28"/>
@@ -2089,7 +2089,7 @@
       <c r="E51" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="F51" s="41"/>
+      <c r="F51" s="38"/>
       <c r="G51" s="25"/>
       <c r="H51" s="29"/>
       <c r="I51" s="26"/>
@@ -2111,7 +2111,7 @@
       <c r="E52" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="F52" s="41"/>
+      <c r="F52" s="38"/>
       <c r="G52" s="24"/>
       <c r="H52" s="23"/>
       <c r="I52" s="28"/>
@@ -2133,7 +2133,7 @@
       <c r="E53" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="F53" s="41"/>
+      <c r="F53" s="38"/>
       <c r="G53" s="25"/>
       <c r="H53" s="29"/>
       <c r="I53" s="26"/>
@@ -2155,7 +2155,7 @@
       <c r="E54" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="F54" s="41"/>
+      <c r="F54" s="38"/>
       <c r="G54" s="25"/>
       <c r="H54" s="29"/>
       <c r="I54" s="26"/>
@@ -2177,7 +2177,7 @@
       <c r="E55" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="F55" s="42"/>
+      <c r="F55" s="39"/>
       <c r="G55" s="24"/>
       <c r="H55" s="23"/>
       <c r="I55" s="28"/>
@@ -2192,11 +2192,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="F43:F55"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="F3:F13"/>
-    <mergeCell ref="A16:F16"/>
-    <mergeCell ref="F18:F26"/>
     <mergeCell ref="G42:I42"/>
     <mergeCell ref="G2:I2"/>
     <mergeCell ref="G17:I17"/>
@@ -2204,6 +2199,11 @@
     <mergeCell ref="A29:F29"/>
     <mergeCell ref="F31:F38"/>
     <mergeCell ref="A41:F41"/>
+    <mergeCell ref="F43:F55"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="F3:F13"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="F18:F26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Grosse mise à jour
</commit_message>
<xml_diff>
--- a/Répartition.xlsx
+++ b/Répartition.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Travail\1er année DUT\Projets\Projet tutoré S2\projetTutS2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F236F1FA-4353-4C27-A4B7-BA0C1A1A82BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB80BFB7-C5CE-4568-BD9D-D68444C90EE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{036A9EC5-0052-46C3-A001-39F17668F270}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="74">
   <si>
     <t>nom</t>
   </si>
@@ -252,13 +252,16 @@
   </si>
   <si>
     <t>∼</t>
+  </si>
+  <si>
+    <t>Reporté</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -293,8 +296,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="21">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -415,6 +425,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -480,7 +496,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -568,22 +584,25 @@
     <xf numFmtId="0" fontId="4" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -594,6 +613,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFCC0000"/>
       <color rgb="FFFFA7A7"/>
       <color rgb="FFF3B6F4"/>
       <color rgb="FFB2EBF8"/>
@@ -603,7 +623,6 @@
       <color rgb="FFF6F6B4"/>
       <color rgb="FFF5CCB5"/>
       <color rgb="FFCD93C5"/>
-      <color rgb="FFF0B290"/>
     </mruColors>
   </colors>
   <extLst>
@@ -916,8 +935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFC8A138-2D9A-4417-92BC-D27501CE0120}">
   <dimension ref="A1:Q56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J44" sqref="J44"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -927,20 +946,20 @@
     <col min="4" max="4" width="14.7109375" customWidth="1"/>
     <col min="5" max="5" width="29.5703125" customWidth="1"/>
     <col min="6" max="6" width="29" customWidth="1"/>
-    <col min="11" max="11" width="10.5703125" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="23" customWidth="1"/>
+    <col min="12" max="12" width="0.140625" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="40" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
       <c r="K1">
         <v>43</v>
       </c>
@@ -968,11 +987,11 @@
       <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="37" t="s">
+      <c r="G2" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
       <c r="J2" s="31" t="s">
         <v>70</v>
       </c>
@@ -997,7 +1016,7 @@
       <c r="E3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="40">
+      <c r="F3" s="38">
         <f>SUM(B3:B13)</f>
         <v>40</v>
       </c>
@@ -1027,12 +1046,12 @@
       <c r="E4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="41"/>
+      <c r="F4" s="39"/>
       <c r="G4" s="25"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
-      <c r="J4" s="36" t="s">
-        <v>72</v>
+      <c r="J4" s="35" t="s">
+        <v>71</v>
       </c>
       <c r="M4" s="27" t="s">
         <v>63</v>
@@ -1054,7 +1073,7 @@
       <c r="E5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="41"/>
+      <c r="F5" s="39"/>
       <c r="G5" s="26"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -1084,12 +1103,12 @@
       <c r="E6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="41"/>
+      <c r="F6" s="39"/>
       <c r="G6" s="23"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
-      <c r="J6" s="36" t="s">
-        <v>72</v>
+      <c r="J6" s="35" t="s">
+        <v>71</v>
       </c>
       <c r="M6" s="30" t="s">
         <v>65</v>
@@ -1114,7 +1133,7 @@
       <c r="E7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="41"/>
+      <c r="F7" s="39"/>
       <c r="G7" s="28"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
@@ -1141,7 +1160,7 @@
       <c r="E8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="41"/>
+      <c r="F8" s="39"/>
       <c r="G8" s="29"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
@@ -1165,7 +1184,7 @@
       <c r="E9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="41"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="26"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
@@ -1189,7 +1208,7 @@
       <c r="E10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="41"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="24"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
@@ -1213,7 +1232,7 @@
       <c r="E11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="41"/>
+      <c r="F11" s="39"/>
       <c r="G11" s="25"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
@@ -1237,11 +1256,14 @@
       <c r="E12" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="41"/>
+      <c r="F12" s="39"/>
       <c r="G12" s="29"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
+      <c r="K12" s="37" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="13" spans="1:17" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
@@ -1259,7 +1281,7 @@
       <c r="E13" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="42"/>
+      <c r="F13" s="40"/>
       <c r="G13" s="28"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
@@ -1268,14 +1290,14 @@
       </c>
     </row>
     <row r="16" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="38" t="s">
+      <c r="A16" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="38"/>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
+      <c r="B16" s="41"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
       <c r="M16" s="22" t="s">
         <v>68</v>
       </c>
@@ -1299,11 +1321,11 @@
       <c r="F17" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G17" s="37" t="s">
+      <c r="G17" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="H17" s="37"/>
-      <c r="I17" s="37"/>
+      <c r="H17" s="43"/>
+      <c r="I17" s="43"/>
       <c r="J17" s="31" t="s">
         <v>70</v>
       </c>
@@ -1327,7 +1349,7 @@
       <c r="E18" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F18" s="39">
+      <c r="F18" s="42">
         <f>SUM(B18:B26)</f>
         <v>24</v>
       </c>
@@ -1357,7 +1379,7 @@
       <c r="E19" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F19" s="39"/>
+      <c r="F19" s="42"/>
       <c r="G19" s="28"/>
       <c r="H19" s="26"/>
       <c r="I19" s="3"/>
@@ -1384,7 +1406,7 @@
       <c r="E20" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="F20" s="39"/>
+      <c r="F20" s="42"/>
       <c r="G20" s="28"/>
       <c r="H20" s="26"/>
       <c r="I20" s="3"/>
@@ -1411,7 +1433,7 @@
       <c r="E21" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="F21" s="39"/>
+      <c r="F21" s="42"/>
       <c r="G21" s="28"/>
       <c r="H21" s="26"/>
       <c r="I21" s="3"/>
@@ -1438,7 +1460,7 @@
       <c r="E22" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="F22" s="39"/>
+      <c r="F22" s="42"/>
       <c r="G22" s="24"/>
       <c r="H22" s="23"/>
       <c r="I22" s="3"/>
@@ -1465,7 +1487,7 @@
       <c r="E23" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="F23" s="39"/>
+      <c r="F23" s="42"/>
       <c r="G23" s="25"/>
       <c r="H23" s="33"/>
       <c r="I23" s="3"/>
@@ -1489,7 +1511,7 @@
       <c r="E24" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="F24" s="39"/>
+      <c r="F24" s="42"/>
       <c r="G24" s="24"/>
       <c r="H24" s="23"/>
       <c r="I24" s="3"/>
@@ -1513,11 +1535,13 @@
       <c r="E25" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F25" s="39"/>
+      <c r="F25" s="42"/>
       <c r="G25" s="24"/>
       <c r="H25" s="23"/>
       <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
+      <c r="J25" s="35" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="26" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
@@ -1535,7 +1559,7 @@
       <c r="E26" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F26" s="39"/>
+      <c r="F26" s="42"/>
       <c r="G26" s="25"/>
       <c r="H26" s="29"/>
       <c r="I26" s="3"/>
@@ -1568,14 +1592,14 @@
       <c r="J28" s="32"/>
     </row>
     <row r="29" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="38" t="s">
+      <c r="A29" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="B29" s="38"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
+      <c r="B29" s="41"/>
+      <c r="C29" s="41"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="41"/>
+      <c r="F29" s="41"/>
       <c r="M29" s="22" t="s">
         <v>68</v>
       </c>
@@ -1599,11 +1623,11 @@
       <c r="F30" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G30" s="37" t="s">
+      <c r="G30" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="H30" s="37"/>
-      <c r="I30" s="37"/>
+      <c r="H30" s="43"/>
+      <c r="I30" s="43"/>
       <c r="J30" s="31" t="s">
         <v>70</v>
       </c>
@@ -1627,7 +1651,7 @@
       <c r="E31" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F31" s="39">
+      <c r="F31" s="42">
         <f>SUM(B31:B38)</f>
         <v>37</v>
       </c>
@@ -1657,7 +1681,7 @@
       <c r="E32" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="F32" s="39"/>
+      <c r="F32" s="42"/>
       <c r="G32" s="25"/>
       <c r="H32" s="29"/>
       <c r="I32" s="28"/>
@@ -1684,7 +1708,7 @@
       <c r="E33" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="F33" s="39"/>
+      <c r="F33" s="42"/>
       <c r="G33" s="25"/>
       <c r="H33" s="29"/>
       <c r="I33" s="28"/>
@@ -1711,7 +1735,7 @@
       <c r="E34" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="F34" s="39"/>
+      <c r="F34" s="42"/>
       <c r="G34" s="24"/>
       <c r="H34" s="23"/>
       <c r="I34" s="26"/>
@@ -1738,11 +1762,13 @@
       <c r="E35" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F35" s="39"/>
+      <c r="F35" s="42"/>
       <c r="G35" s="24"/>
       <c r="H35" s="23"/>
       <c r="I35" s="26"/>
-      <c r="J35" s="3"/>
+      <c r="J35" s="35" t="s">
+        <v>71</v>
+      </c>
       <c r="M35" s="17" t="s">
         <v>66</v>
       </c>
@@ -1763,11 +1789,13 @@
       <c r="E36" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F36" s="39"/>
+      <c r="F36" s="42"/>
       <c r="G36" s="25"/>
       <c r="H36" s="29"/>
       <c r="I36" s="28"/>
-      <c r="J36" s="3"/>
+      <c r="J36" s="35" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="37" spans="1:13" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
@@ -1785,11 +1813,13 @@
       <c r="E37" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F37" s="39"/>
+      <c r="F37" s="42"/>
       <c r="G37" s="24"/>
       <c r="H37" s="23"/>
       <c r="I37" s="26"/>
-      <c r="J37" s="3"/>
+      <c r="J37" s="35" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="38" spans="1:13" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
@@ -1807,11 +1837,14 @@
       <c r="E38" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="F38" s="39"/>
+      <c r="F38" s="42"/>
       <c r="G38" s="24"/>
       <c r="H38" s="23"/>
       <c r="I38" s="26"/>
       <c r="J38" s="3"/>
+      <c r="K38" s="37" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="39" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="8"/>
@@ -1832,14 +1865,14 @@
       <c r="J40" s="32"/>
     </row>
     <row r="41" spans="1:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="38" t="s">
+      <c r="A41" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="B41" s="38"/>
-      <c r="C41" s="38"/>
-      <c r="D41" s="38"/>
-      <c r="E41" s="38"/>
-      <c r="F41" s="38"/>
+      <c r="B41" s="41"/>
+      <c r="C41" s="41"/>
+      <c r="D41" s="41"/>
+      <c r="E41" s="41"/>
+      <c r="F41" s="41"/>
       <c r="G41" s="32"/>
       <c r="H41" s="32"/>
       <c r="I41" s="32"/>
@@ -1867,11 +1900,11 @@
       <c r="F42" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G42" s="37" t="s">
+      <c r="G42" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="H42" s="37"/>
-      <c r="I42" s="37"/>
+      <c r="H42" s="43"/>
+      <c r="I42" s="43"/>
       <c r="J42" s="31" t="s">
         <v>70</v>
       </c>
@@ -1895,7 +1928,7 @@
       <c r="E43" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="F43" s="40">
+      <c r="F43" s="38">
         <f>SUM(B43:B55)</f>
         <v>56</v>
       </c>
@@ -1925,7 +1958,7 @@
       <c r="E44" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="F44" s="41"/>
+      <c r="F44" s="39"/>
       <c r="G44" s="24"/>
       <c r="H44" s="23"/>
       <c r="I44" s="28"/>
@@ -1952,11 +1985,13 @@
       <c r="E45" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="F45" s="41"/>
+      <c r="F45" s="39"/>
       <c r="G45" s="24"/>
       <c r="H45" s="23"/>
       <c r="I45" s="28"/>
-      <c r="J45" s="3"/>
+      <c r="J45" s="35" t="s">
+        <v>71</v>
+      </c>
       <c r="M45" s="20" t="s">
         <v>64</v>
       </c>
@@ -1977,11 +2012,13 @@
       <c r="E46" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="F46" s="41"/>
+      <c r="F46" s="39"/>
       <c r="G46" s="24"/>
       <c r="H46" s="23"/>
       <c r="I46" s="28"/>
-      <c r="J46" s="3"/>
+      <c r="J46" s="35" t="s">
+        <v>71</v>
+      </c>
       <c r="M46" s="30" t="s">
         <v>65</v>
       </c>
@@ -2002,11 +2039,13 @@
       <c r="E47" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="F47" s="41"/>
+      <c r="F47" s="39"/>
       <c r="G47" s="25"/>
       <c r="H47" s="29"/>
       <c r="I47" s="26"/>
-      <c r="J47" s="3"/>
+      <c r="J47" s="36" t="s">
+        <v>72</v>
+      </c>
       <c r="M47" s="17" t="s">
         <v>66</v>
       </c>
@@ -2027,7 +2066,7 @@
       <c r="E48" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="F48" s="41"/>
+      <c r="F48" s="39"/>
       <c r="G48" s="24"/>
       <c r="H48" s="23"/>
       <c r="I48" s="28"/>
@@ -2049,7 +2088,7 @@
       <c r="E49" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="F49" s="41"/>
+      <c r="F49" s="39"/>
       <c r="G49" s="25"/>
       <c r="H49" s="29"/>
       <c r="I49" s="26"/>
@@ -2071,7 +2110,7 @@
       <c r="E50" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="F50" s="41"/>
+      <c r="F50" s="39"/>
       <c r="G50" s="24"/>
       <c r="H50" s="23"/>
       <c r="I50" s="28"/>
@@ -2093,7 +2132,7 @@
       <c r="E51" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="F51" s="41"/>
+      <c r="F51" s="39"/>
       <c r="G51" s="25"/>
       <c r="H51" s="29"/>
       <c r="I51" s="26"/>
@@ -2115,7 +2154,7 @@
       <c r="E52" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="F52" s="41"/>
+      <c r="F52" s="39"/>
       <c r="G52" s="24"/>
       <c r="H52" s="23"/>
       <c r="I52" s="28"/>
@@ -2137,7 +2176,7 @@
       <c r="E53" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="F53" s="41"/>
+      <c r="F53" s="39"/>
       <c r="G53" s="25"/>
       <c r="H53" s="29"/>
       <c r="I53" s="26"/>
@@ -2159,7 +2198,7 @@
       <c r="E54" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="F54" s="41"/>
+      <c r="F54" s="39"/>
       <c r="G54" s="25"/>
       <c r="H54" s="29"/>
       <c r="I54" s="26"/>
@@ -2181,7 +2220,7 @@
       <c r="E55" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="F55" s="42"/>
+      <c r="F55" s="40"/>
       <c r="G55" s="24"/>
       <c r="H55" s="23"/>
       <c r="I55" s="28"/>
@@ -2196,11 +2235,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="F43:F55"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="F3:F13"/>
-    <mergeCell ref="A16:F16"/>
-    <mergeCell ref="F18:F26"/>
     <mergeCell ref="G42:I42"/>
     <mergeCell ref="G2:I2"/>
     <mergeCell ref="G17:I17"/>
@@ -2208,6 +2242,11 @@
     <mergeCell ref="A29:F29"/>
     <mergeCell ref="F31:F38"/>
     <mergeCell ref="A41:F41"/>
+    <mergeCell ref="F43:F55"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="F3:F13"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="F18:F26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>